<commit_message>
update run output only - 4 different settings test
</commit_message>
<xml_diff>
--- a/data/exp_raw/ValBasis2020126.xlsx
+++ b/data/exp_raw/ValBasis2020126.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blomerusjm\.julia\environments\WatVal\LifeVal\data\exp_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9969DBB6-62A6-4499-A345-9C3B277FE114}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5234629A-2F55-4ABD-A6E5-219656904D14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A9C2AE57-0ED9-42B4-9E49-75079AC8A95A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A9C2AE57-0ED9-42B4-9E49-75079AC8A95A}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="57">
   <si>
     <t>runno</t>
   </si>
@@ -189,6 +189,21 @@
   </si>
   <si>
     <t>v5</t>
+  </si>
+  <si>
+    <t>ufs2</t>
+  </si>
+  <si>
+    <t>ufs3</t>
+  </si>
+  <si>
+    <t>ufs4</t>
+  </si>
+  <si>
+    <t>ASSA</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -210,12 +225,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,9 +251,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52A0F44-C1B7-454B-B61E-0EFB69AF87C8}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,10 +616,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9099B4-9B3C-46CC-9511-44FE8A304365}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,17 +755,198 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <v>202012</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="1">INT(RIGHT(E3,2))</f>
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4">
+        <v>202012</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>202012</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00441687-F01A-43D0-9CDE-A695AAE6DD27}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,6 +1164,531 @@
         <v>42</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>